<commit_message>
Fix removing duplicates to prioritize ones with name filled in
</commit_message>
<xml_diff>
--- a/py Sorting and Comparing/testemails_DuplicateFree.xlsx
+++ b/py Sorting and Comparing/testemails_DuplicateFree.xlsx
@@ -462,71 +462,83 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Amy</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Feldkamp</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>251936@dadeschools.net</t>
+          <t>afeldkamp@troy.k12.mi.us</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Kosin</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>204093@dadeschools.net</t>
+          <t>adkosin@clarkston.k12.mi.us</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Elsa</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>273971@dadeschools.net</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>181884@dadeschools.net</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
         <is>
           <t>teacher</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>addison@dadeschools.net</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>administrator</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Kosin</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>adkosin@clarkston.k12.mi.us</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>adsturm@dsdmail.net</t>
+          <t>222963@dadeschools.net</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -537,7 +549,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>adtaylor@dsdmail.net</t>
+          <t>251936@dadeschools.net</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -548,10 +560,14 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>181884@dadeschools.net</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
+          <t>288058@dadeschools.net</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>this@that.com</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>teacher</t>
@@ -563,71 +579,67 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>222963@dadeschools.net</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+          <t>296806@dadeschools.net</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>eat@gmail.com</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>teacher</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Elsa</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Garcia</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>273971@dadeschools.net</t>
+          <t>204093@dadeschools.net</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>teacher</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>288058@dadeschools.net</t>
+          <t>addison@dadeschools.net</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>administrator</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>296806@dadeschools.net</t>
+          <t>adsturm@dsdmail.net</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>staff</t>
-        </is>
-      </c>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Amy</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Feldkamp</t>
-        </is>
-      </c>
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>afeldkamp@troy.k12.mi.us</t>
+          <t>adtaylor@dsdmail.net</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>

</xml_diff>